<commit_message>
finalizando importacion gestion y soporte
</commit_message>
<xml_diff>
--- a/public/instructivo/Instructivo_Carga_Data_Alumnos_Postgrado.xlsx
+++ b/public/instructivo/Instructivo_Carga_Data_Alumnos_Postgrado.xlsx
@@ -365,12 +365,6 @@
 4: Divorsiado (a)</t>
   </si>
   <si>
-    <t>Indicador si el Alumno sufre o no discapacidad. Valores:
-1: Si
-2: No
-Vacío: No</t>
-  </si>
-  <si>
     <t>Discapacidad del Alumno en texto, debe completarse solo si marcó Si a sufre discapacidad (Valor 1)</t>
   </si>
   <si>
@@ -384,12 +378,6 @@
   </si>
   <si>
     <t>¿CUENTA CON ESCALA DE PAGO?</t>
-  </si>
-  <si>
-    <t>Indicador si el Alumno cuenta con una Escala de Pago. Valores:
-1: Si
-2: No
-Vacío: No</t>
   </si>
   <si>
     <t>DESCRIBA ESCALA DE PAGO</t>
@@ -583,6 +571,18 @@
   <si>
     <t>Error en la Columna CORREO ELECTRÓNICO PERSONAL:
 El Valor ingresado se encuentran en blanco, o cuenta con un formato incorrecto. Corrija la Coumna AB, Fila n</t>
+  </si>
+  <si>
+    <t>Indicador si el Alumno sufre o no discapacidad. Valores:
+1: Si
+0: No
+Vacío: No</t>
+  </si>
+  <si>
+    <t>Indicador si el Alumno cuenta con una Escala de Pago. Valores:
+1: Si
+0: No
+Vacío: No</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1136,7 @@
   <dimension ref="A2:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1153,7 @@
   <sheetData>
     <row r="2" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -1260,10 +1260,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>24</v>
@@ -1272,7 +1272,7 @@
         <v>56</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>48</v>
@@ -1281,7 +1281,7 @@
         <v>32</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="93" x14ac:dyDescent="0.35">
@@ -1289,10 +1289,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>24</v>
@@ -1304,13 +1304,13 @@
         <v>65</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>33</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="106.5" x14ac:dyDescent="0.35">
@@ -1339,7 +1339,7 @@
         <v>34</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
@@ -1368,7 +1368,7 @@
         <v>36</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.35">
@@ -1397,7 +1397,7 @@
         <v>37</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="31.5" x14ac:dyDescent="0.35">
@@ -1426,7 +1426,7 @@
         <v>39</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.35">
@@ -1482,7 +1482,7 @@
         <v>43</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
@@ -1511,7 +1511,7 @@
         <v>44</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
@@ -1540,7 +1540,7 @@
         <v>46</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="76.5" x14ac:dyDescent="0.35">
@@ -1569,7 +1569,7 @@
         <v>48</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="61.5" x14ac:dyDescent="0.35">
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>107</v>
+        <v>165</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>38</v>
@@ -1598,7 +1598,7 @@
         <v>49</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.35">
@@ -1609,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>63</v>
@@ -1627,7 +1627,7 @@
         <v>47</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="31.5" x14ac:dyDescent="0.35">
@@ -1635,10 +1635,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>24</v>
@@ -1650,13 +1650,13 @@
         <v>65</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H23" s="16" t="s">
         <v>58</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="21" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1664,10 +1664,10 @@
         <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>113</v>
+        <v>166</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>24</v>
@@ -1685,7 +1685,7 @@
         <v>61</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1693,13 +1693,13 @@
         <v>18</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="D25" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>64</v>
@@ -1708,13 +1708,13 @@
         <v>65</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>52</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="61.5" x14ac:dyDescent="0.35">
@@ -1722,10 +1722,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>24</v>
@@ -1734,7 +1734,7 @@
         <v>68</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G26" s="16">
         <v>15</v>
@@ -1743,7 +1743,7 @@
         <v>54</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="61.5" x14ac:dyDescent="0.35">
@@ -1751,10 +1751,10 @@
         <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>122</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>24</v>
@@ -1763,7 +1763,7 @@
         <v>68</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G27" s="16">
         <v>16</v>
@@ -1772,7 +1772,7 @@
         <v>67</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="121.5" x14ac:dyDescent="0.35">
@@ -1780,10 +1780,10 @@
         <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>24</v>
@@ -1792,7 +1792,7 @@
         <v>23</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G28" s="15">
         <v>4</v>
@@ -1801,7 +1801,7 @@
         <v>55</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
@@ -1830,7 +1830,7 @@
         <v>72</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
@@ -1859,7 +1859,7 @@
         <v>75</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
@@ -1888,7 +1888,7 @@
         <v>79</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
@@ -1917,7 +1917,7 @@
         <v>80</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="61.5" x14ac:dyDescent="0.35">
@@ -1925,10 +1925,10 @@
         <v>26</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>24</v>
@@ -1937,16 +1937,16 @@
         <v>88</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H33" s="16" t="s">
         <v>81</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="31.5" x14ac:dyDescent="0.35">
@@ -1954,10 +1954,10 @@
         <v>27</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>24</v>
@@ -1975,7 +1975,7 @@
         <v>82</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="61.5" x14ac:dyDescent="0.35">
@@ -1983,10 +1983,10 @@
         <v>28</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>24</v>
@@ -2004,7 +2004,7 @@
         <v>83</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="31.5" x14ac:dyDescent="0.35">
@@ -2015,7 +2015,7 @@
         <v>7</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>21</v>

</xml_diff>